<commit_message>
only one question solved
</commit_message>
<xml_diff>
--- a/coding_questions_tracking.xlsx
+++ b/coding_questions_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\Desktop\Coding_Days\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECD6300-BFA3-48EA-8531-FD256569F32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA0880B-7DC4-4C69-9EC0-147F6A19B60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
   <si>
     <t>Date Solved</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>grading problem</t>
+  </si>
+  <si>
+    <t>apple and orange</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/apple-and-orange/problem</t>
   </si>
 </sst>
 </file>
@@ -748,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,6 +1315,23 @@
       </c>
       <c r="H45" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="4">
+        <v>45585</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 8 half done
</commit_message>
<xml_diff>
--- a/coding_questions_tracking.xlsx
+++ b/coding_questions_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\Desktop\Coding_Days\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C646474A-C7F1-4E4B-90F2-F2E8E0552A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533E3A23-3F55-41CF-BCD1-336F30FFD4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="166">
   <si>
     <t>Date Solved</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>search in rotated sorted array</t>
+  </si>
+  <si>
+    <t>koko eating bananas</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/koko-eating-bananas/description/</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G99" sqref="G99"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,6 +2235,26 @@
       </c>
       <c r="H99" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B101" s="4">
+        <v>45660</v>
+      </c>
+      <c r="C101" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101" t="s">
+        <v>90</v>
+      </c>
+      <c r="E101" t="s">
+        <v>47</v>
+      </c>
+      <c r="G101" t="s">
+        <v>91</v>
+      </c>
+      <c r="H101" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>